<commit_message>
Draft of scaling notebook
</commit_message>
<xml_diff>
--- a/data/Self_homodyne_link_loss_sketch.xlsx
+++ b/data/Self_homodyne_link_loss_sketch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santiagoe\OneDrive - Mellanox\Documents\Coherent_project\Swing_considerations\coherent_exercise\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="13_ncr:800001_{10C0D8ED-0E62-4A54-B0ED-37512951C33A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{F587E024-28E3-48D1-B658-58D0A2E7CEE7}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:800001_{10C0D8ED-0E62-4A54-B0ED-37512951C33A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{1ACEA9BC-5298-4EB8-A97A-7BB91A530F16}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D3652AE4-65D7-4D04-BF3D-0B3D3282A9A8}"/>
   </bookViews>
@@ -37,24 +37,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
-    <t>Penalty (dB)</t>
-  </si>
-  <si>
-    <t>S Pav (dBm)</t>
-  </si>
-  <si>
-    <t>LO Pav (dBm)</t>
-  </si>
-  <si>
     <t>Final power</t>
   </si>
   <si>
-    <t>S aggr Penalty (dB)</t>
-  </si>
-  <si>
-    <t>LO aggr Penalty (dB)</t>
-  </si>
-  <si>
     <t>Function</t>
   </si>
   <si>
@@ -166,12 +151,6 @@
     <t>Attach</t>
   </si>
   <si>
-    <t>Splitter (S)</t>
-  </si>
-  <si>
-    <t>Splitter (LO)</t>
-  </si>
-  <si>
     <t>DP IQM</t>
   </si>
   <si>
@@ -194,6 +173,27 @@
   </si>
   <si>
     <t>Hybrid</t>
+  </si>
+  <si>
+    <t>LO Pav</t>
+  </si>
+  <si>
+    <t>LO aggr Penalty</t>
+  </si>
+  <si>
+    <t>Splitter S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Splitter </t>
+  </si>
+  <si>
+    <t>S Pav</t>
+  </si>
+  <si>
+    <t>Penalty</t>
+  </si>
+  <si>
+    <t>S aggr Penalty</t>
   </si>
 </sst>
 </file>
@@ -324,7 +324,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>14</xdr:col>
-          <xdr:colOff>295275</xdr:colOff>
+          <xdr:colOff>142875</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -743,14 +743,14 @@
   <dimension ref="A15:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
     <col min="5" max="5" width="7.140625" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" customWidth="1"/>
@@ -764,51 +764,51 @@
   <sheetData>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" t="s">
         <v>41</v>
       </c>
-      <c r="C15" t="s">
+      <c r="I15" t="s">
         <v>42</v>
       </c>
-      <c r="D15" t="s">
+      <c r="J15" t="s">
         <v>43</v>
       </c>
-      <c r="E15" t="s">
+      <c r="K15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L15" t="s">
         <v>44</v>
       </c>
-      <c r="F15" t="s">
+      <c r="M15" t="s">
+        <v>16</v>
+      </c>
+      <c r="N15" t="s">
         <v>45</v>
       </c>
-      <c r="G15" t="s">
-        <v>46</v>
-      </c>
-      <c r="H15" t="s">
-        <v>48</v>
-      </c>
-      <c r="I15" t="s">
-        <v>49</v>
-      </c>
-      <c r="J15" t="s">
-        <v>50</v>
-      </c>
-      <c r="K15" t="s">
-        <v>47</v>
-      </c>
-      <c r="L15" t="s">
-        <v>51</v>
-      </c>
-      <c r="M15" t="s">
-        <v>21</v>
-      </c>
-      <c r="N15" t="s">
-        <v>52</v>
-      </c>
       <c r="P15" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="B16" s="4">
         <v>16</v>
@@ -867,7 +867,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="5">
@@ -921,7 +921,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="C18" s="3">
         <v>-5</v>
@@ -964,7 +964,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="E20" s="4">
         <f>SUM(C18,E18)</f>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="E21" s="4">
         <f>SUM(C18:D18)</f>
@@ -1062,7 +1062,7 @@
               </from>
               <to>
                 <xdr:col>14</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
+                <xdr:colOff>142875</xdr:colOff>
                 <xdr:row>14</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
@@ -1095,7 +1095,7 @@
   <sheetData>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -1104,24 +1104,24 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -1134,12 +1134,12 @@
         <v>2.7999999999999999E-6</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1152,12 +1152,12 @@
         <v>2.7999999999999999E-6</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1173,7 +1173,7 @@
     </row>
     <row r="8" spans="2:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>14</v>
@@ -1186,12 +1186,12 @@
         <v>2.8000000000000002E-7</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>12</v>
@@ -1204,12 +1204,12 @@
         <v>1.4999999999999999E-7</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1222,12 +1222,12 @@
         <v>1.4000000000000001E-7</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>6</v>
@@ -1240,12 +1240,12 @@
         <v>1.35E-7</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1258,12 +1258,12 @@
         <v>8.7499999999999996E-8</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -1276,12 +1276,12 @@
         <v>3.7E-8</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1296,7 +1296,7 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -1309,12 +1309,12 @@
         <v>1.7079999999999998E-8</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E17" s="10">
         <f>SUM(E5:E15)</f>
@@ -1323,14 +1323,14 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E18" s="10">
         <f>E17*1.25</f>
         <v>8.7207249999999994E-6</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -1341,7 +1341,7 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E21" s="10">
         <f>E20*1000000</f>
@@ -1350,7 +1350,7 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C23">
         <v>4</v>
@@ -1366,7 +1366,7 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -1381,7 +1381,7 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1396,7 +1396,7 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C26">
         <v>8</v>
@@ -1411,7 +1411,7 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E28" s="10">
         <f>SUM(E23:E26)*1000000</f>
@@ -1618,15 +1618,15 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10A797F8-DAB2-47BC-9103-8608BD6CE889}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="34f53576-31fa-4695-b6cf-acc5460440fa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="34f53576-31fa-4695-b6cf-acc5460440fa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Splitting ratio is now -3dB
</commit_message>
<xml_diff>
--- a/data/Self_homodyne_link_loss_sketch.xlsx
+++ b/data/Self_homodyne_link_loss_sketch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santiagoe\OneDrive - Mellanox\Documents\Coherent_project\Swing_considerations\coherent_exercise\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:800001_{10C0D8ED-0E62-4A54-B0ED-37512951C33A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{1ACEA9BC-5298-4EB8-A97A-7BB91A530F16}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="13_ncr:800001_{10C0D8ED-0E62-4A54-B0ED-37512951C33A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BD894032-4483-4B5C-9CFD-BB2D5F26CFA1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D3652AE4-65D7-4D04-BF3D-0B3D3282A9A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D3652AE4-65D7-4D04-BF3D-0B3D3282A9A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -743,7 +745,7 @@
   <dimension ref="A15:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,45 +822,45 @@
       <c r="D16" s="6"/>
       <c r="E16" s="7">
         <f>C16+E18</f>
-        <v>6.2287874528033758</v>
+        <v>8</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" ref="F16:K16" si="0">E16+F18</f>
-        <v>2.2287874528033758</v>
+        <v>4</v>
       </c>
       <c r="G16" s="4">
         <f t="shared" si="0"/>
-        <v>1.2287874528033758</v>
+        <v>3</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="0"/>
-        <v>-0.77121254719662424</v>
+        <v>1</v>
       </c>
       <c r="I16" s="4">
         <f t="shared" si="0"/>
-        <v>-2.7712125471966242</v>
+        <v>-1</v>
       </c>
       <c r="J16" s="4">
         <f t="shared" si="0"/>
-        <v>-4.7712125471966242</v>
+        <v>-3</v>
       </c>
       <c r="K16" s="4">
         <f t="shared" si="0"/>
-        <v>-5.7712125471966242</v>
+        <v>-4</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4">
         <f>K16+S19</f>
-        <v>-5.7712125471966242</v>
+        <v>-4</v>
       </c>
       <c r="N16" s="4">
         <f>M16+N18</f>
-        <v>-12.771212547196624</v>
+        <v>-11</v>
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4">
         <f>N16</f>
-        <v>-12.771212547196624</v>
+        <v>-11</v>
       </c>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
@@ -876,43 +878,43 @@
       </c>
       <c r="D17" s="6">
         <f>C17+D18</f>
-        <v>9.2390874094431865</v>
+        <v>8</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="5"/>
       <c r="G17" s="4">
         <f>D17+G18</f>
-        <v>8.2390874094431865</v>
+        <v>7</v>
       </c>
       <c r="H17" s="5">
         <f>G17+H18</f>
-        <v>6.2390874094431865</v>
+        <v>5</v>
       </c>
       <c r="I17" s="4">
         <f>H17+I18</f>
-        <v>4.2390874094431865</v>
+        <v>3</v>
       </c>
       <c r="J17" s="4">
         <f>I17+J18</f>
-        <v>2.2390874094431865</v>
+        <v>1</v>
       </c>
       <c r="K17" s="4">
         <f>J17+K18</f>
-        <v>1.2390874094431865</v>
+        <v>0</v>
       </c>
       <c r="L17" s="4">
         <f>K17+L18</f>
-        <v>-2.7609125905568135</v>
+        <v>-4</v>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4">
         <f>L17+N18</f>
-        <v>-9.7609125905568135</v>
+        <v>-11</v>
       </c>
       <c r="O17" s="4"/>
       <c r="P17" s="4">
         <f>N17</f>
-        <v>-9.7609125905568135</v>
+        <v>-11</v>
       </c>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
@@ -927,12 +929,10 @@
         <v>-5</v>
       </c>
       <c r="D18" s="1">
-        <f>LOG10(2/3)*10</f>
-        <v>-1.7609125905568126</v>
+        <v>-3</v>
       </c>
       <c r="E18" s="2">
-        <f>LOG10(1/3)*10</f>
-        <v>-4.7712125471966242</v>
+        <v>-3</v>
       </c>
       <c r="F18" s="5">
         <v>-4</v>
@@ -968,40 +968,40 @@
       </c>
       <c r="E20" s="4">
         <f>SUM(C18,E18)</f>
-        <v>-9.7712125471966242</v>
+        <v>-8</v>
       </c>
       <c r="F20" s="4">
         <f t="shared" ref="F20:K20" si="1">E20+F18</f>
-        <v>-13.771212547196624</v>
+        <v>-12</v>
       </c>
       <c r="G20" s="4">
         <f t="shared" si="1"/>
-        <v>-14.771212547196624</v>
+        <v>-13</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" si="1"/>
-        <v>-16.771212547196626</v>
+        <v>-15</v>
       </c>
       <c r="I20" s="4">
         <f t="shared" si="1"/>
-        <v>-18.771212547196626</v>
+        <v>-17</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" si="1"/>
-        <v>-20.771212547196626</v>
+        <v>-19</v>
       </c>
       <c r="K20" s="4">
         <f t="shared" si="1"/>
-        <v>-21.771212547196626</v>
+        <v>-20</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4">
         <f>K20+M18</f>
-        <v>-25.271212547196626</v>
+        <v>-23.5</v>
       </c>
       <c r="N20" s="4">
         <f>M20+N18</f>
-        <v>-32.271212547196626</v>
+        <v>-30.5</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
@@ -1010,37 +1010,37 @@
       </c>
       <c r="E21" s="4">
         <f>SUM(C18:D18)</f>
-        <v>-6.7609125905568126</v>
+        <v>-8</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4">
         <f>E21+G18</f>
-        <v>-7.7609125905568126</v>
+        <v>-9</v>
       </c>
       <c r="H21" s="4">
         <f>G21+H18</f>
-        <v>-9.7609125905568135</v>
+        <v>-11</v>
       </c>
       <c r="I21" s="4">
         <f>H21+I18</f>
-        <v>-11.760912590556813</v>
+        <v>-13</v>
       </c>
       <c r="J21" s="4">
         <f>I21+J18</f>
-        <v>-13.760912590556813</v>
+        <v>-15</v>
       </c>
       <c r="K21" s="4">
         <f>J21+K18</f>
-        <v>-14.760912590556813</v>
+        <v>-16</v>
       </c>
       <c r="L21" s="4">
         <f>K21+L18</f>
-        <v>-18.760912590556813</v>
+        <v>-20</v>
       </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4">
         <f>L21+N18</f>
-        <v>-25.760912590556813</v>
+        <v>-27</v>
       </c>
     </row>
   </sheetData>
@@ -1461,21 +1461,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100618960C626218945AD5E02DF4EE0DE37" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f131c94f27f7306b854c3d534882a70">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="34f53576-31fa-4695-b6cf-acc5460440fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d63c241fda5111873f75e13a10882e88" ns2:_="">
     <xsd:import namespace="34f53576-31fa-4695-b6cf-acc5460440fa"/>
@@ -1607,10 +1592,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14CDBCC6-D225-40D4-9956-6B4EB0957DBD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30B1C44B-6DCE-4743-8607-AC99C3A5D839}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="34f53576-31fa-4695-b6cf-acc5460440fa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1632,19 +1642,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30B1C44B-6DCE-4743-8607-AC99C3A5D839}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14CDBCC6-D225-40D4-9956-6B4EB0957DBD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="34f53576-31fa-4695-b6cf-acc5460440fa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>